<commit_message>
Updated all criteria functions
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>technical_skill</t>
+          <t>skill_group</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -501,22 +501,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ang Teik Hun</t>
+          <t>GOO YE JUI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+60124773683</t>
+          <t>+60184040438</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>teikhun0422@hotmail.com</t>
+          <t>yjyejui626@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -526,102 +526,37 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['Country: Malaysia', 'State: Penang', 'City: Butterworth']</t>
+          <t>[{'Country': 'Malaysia', 'State': 'Penang', 'City': 'Bukit Mertajam'}]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Applied Data Analytics', 'level': "Master's", 'cgpa': '6.42', 'university': 'Australian National University', 'Start Date': '2021-07', 'Year of Graduation': '2022'}]</t>
+          <t>[{'field_of_study': 'Bachelor Of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.97', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': '2024'}, {'field_of_study': 'Foundation in Science', 'level': 'Foundation', 'cgpa': '3.78', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2019', 'year_of_graduation': '2020'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['Microsoft Certified: Azure Fundamentals', 'Microsoft Certified: Azure AI Engineer Associate']</t>
+          <t>['Microsoft Certified: Azure AI Fundamentals', 'Google Data Analytics Certificate by Coursera', 'Alteryx Foundational Micro-Credential', 'Alteryx Designer Core Certification', 'AWS Academy Graduate - AWS Academy Cloud Foundations', 'AWS Academy Graduate - AWS Academy Machine Learning Foundations', 'AWS Academy Graduate - AWS Academy Data Analytics', 'AWS Academy Graduate - AWS Academy Machine Learning for Natural Language Processing', 'AWS Academy Graduate - AWS Academy Data Engineering', 'AWS Academy Graduate - AWS Academy Cloud Web Application Builder', 'AWS Academy Graduate - AWS Academy Cloud Data Pipeline Builder']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Python', 'R', 'SQL']</t>
+          <t>['Full-stack web development', 'Natural Language Processing', 'Generative AI']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['Power BI']</t>
+          <t>['HTML 5', 'CSS', 'JavaScript', 'PHP', 'SQL', 'Python', '.NET', 'React', 'spaCy', 'NLTK', 'TensorFlow', 'PyTorch', 'LangChain', 'Llama', 'Django', 'PostgreSQL', 'OpenAI GPT', 'Laravel', 'MySQL', 'Microsoft SQL Server', '.NET MVC Framework']</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['English', 'Mandarin', 'Malay', 'French']</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Data Scientist', 'job_company': 'Petroliam Nasional Berhad', 'Industries': 'Oil and Gas', 'start_date': '2020-11', 'end_date': '2021-07', 'job_location': 'KL', 'Job Duration (Years)': 0.6}, {'job_title': 'Tutor', 'job_company': 'Australian National University', 'Industries': 'Education', 'start_date': '2022-06', 'end_date': '2022-12', 'job_location': 'Canberra', 'Job Duration (Years)': 0.5}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>GOO YE JUI</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>+60184040438</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>yjyejui626@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>['Country: Malaysia', 'State: Penang', 'City: Bukit Mertajam']</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>[{'field_of_study': 'Bachelor Of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.97', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': '2024'}, {'field_of_study': 'Foundation in Science', 'level': 'Foundation', 'cgpa': '3.78', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2019', 'year_of_graduation': '2020'}]</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>['Microsoft Certified: Azure AI Fundamentals', 'Google Data Analytics Certificate by Coursera', 'Alteryx Foundational Micro-Credential', 'Alteryx Designer Core Certification', 'AWS Academy Graduate - AWS Academy Cloud Foundations', 'AWS Academy Graduate - AWS Academy Machine Learning Foundations', 'AWS Academy Graduate - AWS Academy Data Analytics', 'AWS Academy Graduate - AWS Academy Machine Learning for Natural Language Processing', 'AWS Academy Graduate - AWS Academy Data Engineering', 'AWS Academy Graduate - AWS Academy Cloud Web Application Builder', 'AWS Academy Graduate - AWS Academy Cloud Data Pipeline Builder']</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>['Full-stack web development (HTML 5, CSS, JavaScript, PHP, SQL, Python, .NET, React)', 'Natural Language Processing: spaCy, NLTK, TensorFlow, PyTorch', 'Generative AI related: LangChain, Llama']</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>['English', 'Mandarin', 'Malay', 'French']</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>[{'job_title': 'Data Science Intern', 'job_company': 'Petronas Digital Sdn Bhd', 'industry': 'Information Technology', 'start_date': '2023-09', 'end_date': '2024-06', 'job_location': 'N/A'}]</t>
+          <t>[{'job_title': 'Data Science Intern', 'job_company': 'Petronas Digital Sdn Bhd', 'Industries': 'Information Technology', 'start_date': '2023-09', 'end_date': '2024-06', 'job_location': 'N/A'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated evaluation criteria pipeline
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,12 +526,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{'Country': 'Malaysia', 'State': 'Penang', 'City': 'Bukit Mertajam'}]</t>
+          <t>['', 'Penang', 'Bukit Mertajam']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Bachelor Of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.97', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020-09-01', 'year_of_graduation': '2024'}, {'field_of_study': 'Foundation in Science', 'level': 'Foundation', 'cgpa': '3.78', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2019-09-01', 'year_of_graduation': '2020'}]</t>
+          <t>[{'field_of_study': 'Bachelor Of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.97', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': '2024'}, {'field_of_study': 'Foundation in Science', 'level': 'Foundation', 'cgpa': '3.78', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2019', 'year_of_graduation': '2020'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -541,12 +541,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Full-stack web development', 'Natural Language Processing', 'Generative AI']</t>
+          <t>['Time Management', 'Collaboration', 'Adaptability', 'Leadership', 'Communication']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['HTML 5', 'CSS', 'JavaScript', 'PHP', 'SQL', 'Python', '.NET', 'React', 'spaCy', 'NLTK', 'TensorFlow', 'PyTorch', 'LangChain', 'Llama', 'Django', 'PostgreSQL', 'MongoDB', 'Laravel', 'MySQL', 'Microsoft SQL Server', '.NET MVC Framework']</t>
+          <t>['HTML 5', 'CSS', 'JavaScript', 'PHP', 'SQL', 'Python', '.NET', 'React', 'spaCy', 'NLTK', 'TensorFlow', 'PyTorch', 'LangChain', 'Llama', 'Django', 'PostgreSQL', 'Laravel', 'MySQL', 'Microsoft SQL Server', '.NET MVC Framework']</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -556,7 +556,72 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Data Science Intern', 'job_company': 'Petronas Digital Sdn Bhd', 'Industries': 'Information Technology', 'start_date': '2023-09-01', 'end_date': '2024-06-01', 'job_location': 'N/A'}]</t>
+          <t>[{'job_title': 'Data Science Intern', 'job_company': 'Petronas Digital Sdn Bhd', 'Industries': 'Oil &amp; Gas', 'start_date': '2023-09', 'end_date': '2024-06', 'job_location': 'Bukit Mertajam, Penang'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ang Teik Hun</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>+60124773683</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>teikhun0422@hotmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[{'Country': 'Malaysia', 'State': 'Penang', 'City': 'Butterworth'}]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[{'field_of_study': 'Applied Data Analytics', 'level': "Master's", 'cgpa': '6.42/7', 'university': 'Australian National University', 'start_date': '2021-07', 'year_of_graduation': '2022'}]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>['Microsoft Certified: Azure Fundamentals', 'Microsoft Certified: Azure AI Engineer Associate']</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>['Analytical Thinking Skills', 'Adaptability', 'Time Management', 'Leadership', 'Power BI', 'Python', 'Neural Network', 'Machine Learning (SKlearn)', 'Database SQL', 'Data Wrangling', 'Optimization']</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>['N/A']</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>['Chinese', 'English', 'Malay', 'French']</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>[{'job_title': 'Data Scientist', 'job_company': 'Petroliam Nasional Berhad Group Digital', 'Industries': 'Oil &amp; Gas', 'start_date': '2020-11', 'end_date': '2021-07', 'job_location': 'KL', 'job_duration': '0.6'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Prompt tuned extract_information 2. Updated chat with pandas dataframe. 3. Update default chat with readme
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -501,17 +501,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GOO YE JUI</t>
+          <t>Farhan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+60184040438</t>
+          <t>+60177496576</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>yjyejui626@gmail.com</t>
+          <t>farhan257@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -526,37 +526,37 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['', 'Penang', 'Bukit Mertajam']</t>
+          <t>[{'Country': '', 'State': 'Kuala Lumpur', 'City': ''}]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Bachelor Of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.97', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': '2024'}, {'field_of_study': 'Foundation in Science', 'level': 'Foundation', 'cgpa': '3.78', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2019', 'year_of_graduation': '2020'}]</t>
+          <t>[{'field_of_study': 'Software Engineering', 'level': 'Bachelor', 'cgpa': '3.54', 'university': 'Universiti Teknologi Malaysia (UTM)', 'start_date': 'N/A', 'year_of_graduation': 'N/A'}, {'field_of_study': 'Software Engineering', 'level': 'Master of Software Engineering', 'cgpa': '3.98', 'university': 'Universiti Teknologi Malaysia (UTM)', 'start_date': 'N/A', 'year_of_graduation': 'N/A'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['Microsoft Certified: Azure AI Fundamentals', 'Google Data Analytics Certificate by Coursera', 'Alteryx Foundational Micro-Credential', 'Alteryx Designer Core Certification', 'AWS Academy Graduate - AWS Academy Cloud Foundations', 'AWS Academy Graduate - AWS Academy Machine Learning Foundations', 'AWS Academy Graduate - AWS Academy Data Analytics', 'AWS Academy Graduate - AWS Academy Machine Learning for Natural Language Processing', 'AWS Academy Graduate - AWS Academy Data Engineering', 'AWS Academy Graduate - AWS Academy Cloud Web Application Builder', 'AWS Academy Graduate - AWS Academy Cloud Data Pipeline Builder']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Time Management', 'Collaboration', 'Adaptability', 'Leadership', 'Communication']</t>
+          <t>['Agile Software Development', 'Requirement analysis', 'DevOps', 'Linux/Unix environment', 'CI/CD pipeline (Jenkins)', 'Containerization (Kubernetes &amp; Docker)', 'Git (Git Bash, GitHub, GitLab)', 'Software Architecture &amp; Design', 'Software Testing (Cucumber, JMeter)', 'Virtualization (VMWare/VirtualBox)', 'Software Documentation', 'Software Standards (ISO/IEC/IEEE)', 'SQL Server Management', 'Laravel', 'Azure', 'Programming Languages (Java, PHP, C++, SQL, JavaScript, Python)', 'Web Development', 'Microsoft Office', 'Enterprise Architect', 'Epicor', 'Visual Studio, Android Studio, Eclipse, Spring Tool Suite, Ionic', 'Wireshark/Tshark']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['HTML 5', 'CSS', 'JavaScript', 'PHP', 'SQL', 'Python', '.NET', 'React', 'spaCy', 'NLTK', 'TensorFlow', 'PyTorch', 'LangChain', 'Llama', 'Django', 'PostgreSQL', 'Laravel', 'MySQL', 'Microsoft SQL Server', '.NET MVC Framework']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['English', 'Mandarin', 'Malay', 'French']</t>
+          <t>['English', 'Bahasa Malaysia']</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Data Science Intern', 'job_company': 'Petronas Digital Sdn Bhd', 'Industries': 'Oil &amp; Gas', 'start_date': '2023-09', 'end_date': '2024-06', 'job_location': 'Bukit Mertajam, Penang'}]</t>
+          <t>[{'job_title': 'Consultant', 'job_company': 'Finsoft Consulting Sdn Bhd', 'Industries': 'N/A', 'start_date': '2022-04-01', 'end_date': '2022-07-01', 'job_location': 'N/A'}, {'job_title': 'Software Engineer', 'job_company': 'Axacute', 'Industries': 'N/A', 'start_date': '2020-07-01', 'end_date': '2021-10-01', 'job_location': 'N/A'}, {'job_title': 'Intern', 'job_company': 'Openet', 'Industries': 'N/A', 'start_date': '2019-07-01', 'end_date': '2019-12-01', 'job_location': 'N/A'}]</t>
         </is>
       </c>
     </row>
@@ -566,22 +566,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ang Teik Hun</t>
+          <t>MOHAMAD AMIR AFIFIE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>+60124773683</t>
+          <t>0111 - 488 3732</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>teikhun0422@hotmail.com</t>
+          <t>amirafifie@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -591,37 +591,37 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[{'Country': 'Malaysia', 'State': 'Penang', 'City': 'Butterworth'}]</t>
+          <t>['Malaysia', 'Cyberjaya', '']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Applied Data Analytics', 'level': "Master's", 'cgpa': '6.42/7', 'university': 'Australian National University', 'start_date': '2021-07', 'year_of_graduation': '2022'}]</t>
+          <t>[{'field_of_study': 'Computer Science', 'level': "Bachelor's Degree", 'cgpa': 'N/A', 'university': 'NATIONAL UNIVERSITY OF MALAYSIA', 'start_date': '2017', 'year_of_graduation': '2021'}, {'field_of_study': 'Science', 'level': 'Foundation', 'cgpa': 'N/A', 'university': 'UNIVERSITI TEKNOLOGI MARA', 'start_date': '2016', 'year_of_graduation': '2017'}]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['Microsoft Certified: Azure Fundamentals', 'Microsoft Certified: Azure AI Engineer Associate']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Analytical Thinking Skills', 'Adaptability', 'Time Management', 'Leadership', 'Power BI', 'Python', 'Neural Network', 'Machine Learning (SKlearn)', 'Database SQL', 'Data Wrangling', 'Optimization']</t>
+          <t>['Data Visualisation', 'Machine Learning', 'Data Analysis', 'Python', 'Java', 'SQL', 'C', 'VBA', 'Power BI', 'Excel', 'Scikit-learn', 'NLTK', 'Vader', 'Textblob', 'Pandas', 'Matplotlib', 'Numpy', 'Problem-Solving', 'Team Player', 'Communication']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>['N/A']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>['Chinese', 'English', 'Malay', 'French']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Data Scientist', 'job_company': 'Petroliam Nasional Berhad Group Digital', 'Industries': 'Oil &amp; Gas', 'start_date': '2020-11', 'end_date': '2021-07', 'job_location': 'KL', 'job_duration': '0.6'}]</t>
+          <t>[{'job_title': 'HR DATA ANALYST INTERN', 'job_company': 'Safran Landing System', 'Industries': 'N/A', 'start_date': '2022-08-01', 'end_date': '2023-01-31', 'job_location': 'N/A', 'job_duration': 0.42}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Modified Candidate class metadata for prompts
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -501,62 +501,62 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Farhan</t>
+          <t>MOHD ARIFFIN BIN AHMAD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+60177496576</t>
+          <t>+6013- 8693559</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>farhan257@gmail.com</t>
+          <t>ariffinahmad1994@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{'Country': '', 'State': 'Kuala Lumpur', 'City': ''}]</t>
+          <t>['Malaysia', 'Sabah', 'Tawau']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Software Engineering', 'level': 'Bachelor', 'cgpa': '3.54', 'university': 'Universiti Teknologi Malaysia (UTM)', 'start_date': 'N/A', 'year_of_graduation': 'N/A'}, {'field_of_study': 'Software Engineering', 'level': 'Master of Software Engineering', 'cgpa': '3.98', 'university': 'Universiti Teknologi Malaysia (UTM)', 'start_date': 'N/A', 'year_of_graduation': 'N/A'}]</t>
+          <t>[{'field_of_study': 'Geology', 'level': "Bachelor's Degree", 'cgpa': 'N/A', 'university': 'Universiti Malaysia Sabah', 'start_date': '2013-09-01', 'year_of_graduation': '2016'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>['PTW Level 1 (INSTEP)', 'PTW Level 2 (INSTEP)', 'OGSP (NIOSH)', 'First Aid Training (Red Crescent, Miri)', 'Basic Fire Fighting Training (Bomba, Lintas)', 'CIDB']</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>['N/A']</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>['AutoCAD 20 21', 'CorelDRAW X7', 'ArcGIS (Basic)', 'Surfer', 'GCDkit', 'Ilwis', 'Microsoft Office']</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>['Agile Software Development', 'Requirement analysis', 'DevOps', 'Linux/Unix environment', 'CI/CD pipeline (Jenkins)', 'Containerization (Kubernetes &amp; Docker)', 'Git (Git Bash, GitHub, GitLab)', 'Software Architecture &amp; Design', 'Software Testing (Cucumber, JMeter)', 'Virtualization (VMWare/VirtualBox)', 'Software Documentation', 'Software Standards (ISO/IEC/IEEE)', 'SQL Server Management', 'Laravel', 'Azure', 'Programming Languages (Java, PHP, C++, SQL, JavaScript, Python)', 'Web Development', 'Microsoft Office', 'Enterprise Architect', 'Epicor', 'Visual Studio, Android Studio, Eclipse, Spring Tool Suite, Ionic', 'Wireshark/Tshark']</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>['English', 'Bahasa Malaysia']</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Consultant', 'job_company': 'Finsoft Consulting Sdn Bhd', 'Industries': 'N/A', 'start_date': '2022-04-01', 'end_date': '2022-07-01', 'job_location': 'N/A'}, {'job_title': 'Software Engineer', 'job_company': 'Axacute', 'Industries': 'N/A', 'start_date': '2020-07-01', 'end_date': '2021-10-01', 'job_location': 'N/A'}, {'job_title': 'Intern', 'job_company': 'Openet', 'Industries': 'N/A', 'start_date': '2019-07-01', 'end_date': '2019-12-01', 'job_location': 'N/A'}]</t>
+          <t>[{'job_title': 'Geologist', 'job_company': 'SATOK BRIDGE AREA CONSULTING ENGINEERS SDN. BHD.', 'Industries': 'Engineering', 'start_date': '2020-11-01', 'end_date': '2024-05-15'}, {'job_title': 'Geologist', 'job_company': 'SATOK BRIDGE AREA CONSULTING ENGINEERS SDN. BHD.', 'Industries': 'Engineering', 'start_date': '2020-02-01', 'end_date': '2020-10-01'}, {'job_title': 'Project Coordinator', 'job_company': 'MAJUMEC BINA SDN. BHD.', 'Industries': 'Construction', 'start_date': '2018-05-01', 'end_date': '2020-01-01'}, {'job_title': 'Engineering Geologist', 'job_company': 'MAJUMEC BINA SDN. BHD.', 'Industries': 'Construction', 'start_date': '2017-08-01', 'end_date': '2018-04-01'}, {'job_title': 'Junior Geologist', 'job_company': 'GEOSPEC SDN. BHD.', 'Industries': 'Geology', 'start_date': '2016-07-01', 'end_date': '2016-09-01'}]</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MOHAMAD AMIR AFIFIE</t>
+          <t>DARIN NUR ADLEEN BINTI ROSALIZI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0111 - 488 3732</t>
+          <t>+6019 353 -4359</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>amirafifie@gmail.com</t>
+          <t>darinrosalizi@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -591,12 +591,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['Malaysia', 'Cyberjaya', '']</t>
+          <t>['Malaysia', 'Selangor', 'Sungai Buloh']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Computer Science', 'level': "Bachelor's Degree", 'cgpa': 'N/A', 'university': 'NATIONAL UNIVERSITY OF MALAYSIA', 'start_date': '2017', 'year_of_graduation': '2021'}, {'field_of_study': 'Science', 'level': 'Foundation', 'cgpa': 'N/A', 'university': 'UNIVERSITI TEKNOLOGI MARA', 'start_date': '2016', 'year_of_graduation': '2017'}]</t>
+          <t>[{'field_of_study': 'Intelligent Systems Engineering', 'level': 'Bachelor of Information Systems (Honors)', 'cgpa': '3.67', 'university': 'UiTM Shah Alam', 'start_date': '2020-03', 'year_of_graduation': '2022'}, {'field_of_study': 'Computer Science', 'level': 'Diploma', 'cgpa': '3.67', 'university': 'UiTM Segamat', 'start_date': '2017-05', 'year_of_graduation': '2020'}]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Data Visualisation', 'Machine Learning', 'Data Analysis', 'Python', 'Java', 'SQL', 'C', 'VBA', 'Power BI', 'Excel', 'Scikit-learn', 'NLTK', 'Vader', 'Textblob', 'Pandas', 'Matplotlib', 'Numpy', 'Problem-Solving', 'Team Player', 'Communication']</t>
+          <t>['Requirement Analysis', 'Technical Documentation', 'Agile Methodologies', 'Project Management', 'Process Flow Diagrams']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['English', 'Malay']</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[{'job_title': 'HR DATA ANALYST INTERN', 'job_company': 'Safran Landing System', 'Industries': 'N/A', 'start_date': '2022-08-01', 'end_date': '2023-01-31', 'job_location': 'N/A', 'job_duration': 0.42}]</t>
+          <t>[{'job_title': 'System Analyst', 'job_company': 'Artanis Cloud Sdn Bhd', 'Industries': 'Information Technology', 'start_date': '2022-03', 'end_date': '2022-08', 'job_location': 'Shah Alam, Selangor'}, {'job_title': 'System Analyst', 'job_company': 'Artanis Cloud Sdn Bhd', 'Industries': 'Information Technology', 'start_date': '2022-09', 'end_date': '2023-01', 'job_location': 'Shah Alam, Selangor'}, {'job_title': 'Sales Associate', 'job_company': 'TS Concept Store', 'Industries': 'Retail', 'start_date': '2017-02', 'end_date': '2017-04', 'job_location': 'Sungai Buloh, Selangor'}, {'job_title': 'System Developer', 'job_company': 'SIRIM Berhad', 'Industries': 'Research and Development', 'start_date': '2019-07', 'end_date': '2019-09', 'job_location': 'Shah Alam, Selangor'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add regex to education_background, current_location
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -501,17 +501,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MOHD ARIFFIN BIN AHMAD</t>
+          <t>Nor Shahirah Shaik Amir</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+6013- 8693559</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ariffinahmad1994@gmail.com</t>
+          <t>shahirahshaik25@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -526,37 +526,37 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['Malaysia', 'Sabah', 'Tawau']</t>
+          <t>['Malaysia', 'Selangor', 'Sepang']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Geology', 'level': "Bachelor's Degree", 'cgpa': 'N/A', 'university': 'Universiti Malaysia Sabah', 'start_date': '2013-09-01', 'year_of_graduation': '2016'}]</t>
+          <t>[['Electric, Electronics &amp; System Engineering (Image processing)', 'Master of Science', 'N/A', 'Universiti Kebangsaan Malaysia', '2015-2019'], ['Electric, Electronics &amp; System Engineering (Communication &amp; Computer)', "Bachelor's degree", 'N/A', 'Universiti Kebangsaan Malaysia', '2009-2013'], ['Science majoring in Biology', 'Matriculation', 'N/A', 'Penang Matriculation College', '2008-2009']]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['PTW Level 1 (INSTEP)', 'PTW Level 2 (INSTEP)', 'OGSP (NIOSH)', 'First Aid Training (Red Crescent, Miri)', 'Basic Fire Fighting Training (Bomba, Lintas)', 'CIDB']</t>
+          <t>['Google Data Analytics Professional Certificate']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>['SQL', 'R (Programming Language)', 'Data Analytics', 'Project Planning', 'Google Sheets', 'Data Analysis', 'Research and Development (R&amp;D)', 'Professional Communication', 'Program Management', 'C (Programming Language)']</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>['MATLAB', 'Python', 'R', 'SQL', 'Microsoft Word', 'Microsoft PowerPoint', 'Microsoft Excel', 'Microsoft Access', 'Microsoft Publisher', 'Google Docs', 'Google Sheets', 'Google Slides', 'Google Form', 'MPLAB', 'Arduino IDE', 'Visual Studio Code IDE', 'MIT App Inventor', 'Filmora 9', 'SPSS']</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>['N/A']</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>['AutoCAD 20 21', 'CorelDRAW X7', 'ArcGIS (Basic)', 'Surfer', 'GCDkit', 'Ilwis', 'Microsoft Office']</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'Geologist', 'job_company': 'SATOK BRIDGE AREA CONSULTING ENGINEERS SDN. BHD.', 'Industries': 'Engineering', 'start_date': '2020-11-01', 'end_date': '2024-05-15'}, {'job_title': 'Geologist', 'job_company': 'SATOK BRIDGE AREA CONSULTING ENGINEERS SDN. BHD.', 'Industries': 'Engineering', 'start_date': '2020-02-01', 'end_date': '2020-10-01'}, {'job_title': 'Project Coordinator', 'job_company': 'MAJUMEC BINA SDN. BHD.', 'Industries': 'Construction', 'start_date': '2018-05-01', 'end_date': '2020-01-01'}, {'job_title': 'Engineering Geologist', 'job_company': 'MAJUMEC BINA SDN. BHD.', 'Industries': 'Construction', 'start_date': '2017-08-01', 'end_date': '2018-04-01'}, {'job_title': 'Junior Geologist', 'job_company': 'GEOSPEC SDN. BHD.', 'Industries': 'Geology', 'start_date': '2016-07-01', 'end_date': '2016-09-01'}]</t>
+          <t>[{'job_title': 'Media Officer', 'job_company': 'Pertubuhan IKRAM Malaysia', 'Industries': 'Media', 'start_date': '2021-04', 'end_date': 'Present', 'job_location': 'N/A', 'job_duration': 1.92}, {'job_title': 'Research Officer', 'job_company': 'UKM', 'Industries': 'Research', 'start_date': '2019-04', 'end_date': '2020-08', 'job_location': 'N/A', 'job_duration': 1.42}, {'job_title': 'Research Assistant', 'job_company': 'UKM', 'Industries': 'Research', 'start_date': '2014-04', 'end_date': '2015-07', 'job_location': 'N/A', 'job_duration': 1.33}, {'job_title': 'Internship', 'job_company': 'Astana Digital Sdn. Bhd', 'Industries': 'N/A', 'start_date': '2012-06', 'end_date': '2012-09', 'job_location': 'N/A', 'job_duration': 0.33}]</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DARIN NUR ADLEEN BINTI ROSALIZI</t>
+          <t>ELNI FATIENY BINTI MOHD SALMI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>+6019 353 -4359</t>
+          <t>011-13244806</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>darinrosalizi@gmail.com</t>
+          <t>elnifatieny136@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -591,37 +591,37 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['Malaysia', 'Selangor', 'Sungai Buloh']</t>
+          <t>['Malaysia', 'N/A', 'N/A']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Intelligent Systems Engineering', 'level': 'Bachelor of Information Systems (Honors)', 'cgpa': '3.67', 'university': 'UiTM Shah Alam', 'start_date': '2020-03', 'year_of_graduation': '2022'}, {'field_of_study': 'Computer Science', 'level': 'Diploma', 'cgpa': '3.67', 'university': 'UiTM Segamat', 'start_date': '2017-05', 'year_of_graduation': '2020'}]</t>
+          <t>[{'field_of_study': 'Information System', 'level': 'Bachelor of Science', 'cgpa': '3.53', 'university': 'Universiti Teknologi Petronas', 'start_date': '2018-05', 'year_of_graduation': '2021'}]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['N/A']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Requirement Analysis', 'Technical Documentation', 'Agile Methodologies', 'Project Management', 'Process Flow Diagrams']</t>
+          <t>['Data Analyst', 'Corporate Management', 'Software Designing', 'Project Management', 'Marketing Operation']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Eclipse', 'Anaconda', 'R studio', 'Android Studio', 'PowerBI', 'Firebase', 'Visual Studio Code', 'Microsoft Office', 'Google Collab', 'Oracle Live', 'phpMyAdmin', 'MySQL', 'SQL Server Management Studio', 'WinSCP', 'Salesforce', 'WordPress']</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>['English', 'Malay']</t>
+          <t>['Malay', 'English']</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[{'job_title': 'System Analyst', 'job_company': 'Artanis Cloud Sdn Bhd', 'Industries': 'Information Technology', 'start_date': '2022-03', 'end_date': '2022-08', 'job_location': 'Shah Alam, Selangor'}, {'job_title': 'System Analyst', 'job_company': 'Artanis Cloud Sdn Bhd', 'Industries': 'Information Technology', 'start_date': '2022-09', 'end_date': '2023-01', 'job_location': 'Shah Alam, Selangor'}, {'job_title': 'Sales Associate', 'job_company': 'TS Concept Store', 'Industries': 'Retail', 'start_date': '2017-02', 'end_date': '2017-04', 'job_location': 'Sungai Buloh, Selangor'}, {'job_title': 'System Developer', 'job_company': 'SIRIM Berhad', 'Industries': 'Research and Development', 'start_date': '2019-07', 'end_date': '2019-09', 'job_location': 'Shah Alam, Selangor'}]</t>
+          <t>[{'job_title': 'Marketing Associate Operation', 'job_company': '2X Marketing Sdn Bhd', 'Industries': 'Marketing', 'start_date': '2022-09', 'end_date': '2024-05-15'}, {'job_title': 'Software Engineer', 'job_company': 'ManagePay System Berhad', 'Industries': 'Finance', 'start_date': '2022-01', 'end_date': '2024-05-15'}, {'job_title': 'Change Management Intern', 'job_company': 'Petroliam Nasional Berhad', 'Industries': 'Oil &amp; Gas', 'start_date': '2020-01', 'end_date': '2020-09'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update post evaluation rag
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,37 +461,32 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>previous_job_roles</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>current_location</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>education_background</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>professional_certificate</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>skill_group</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>technology_programs_tool</t>
-        </is>
-      </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
           <t>language</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>previous_job_roles</t>
         </is>
       </c>
     </row>
@@ -501,62 +496,57 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nor Shahirah Shaik Amir</t>
+          <t>NURUL SHAHIRAH BINTI MOHD IDRIS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>+6013 3872826</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>shahirahidris98@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>shahirahshaik25@gmail.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['Malaysia', 'Selangor', 'Sepang']</t>
+          <t>[{'job_title': 'Market Research Analyst', 'job_company': 'MANPOWER GROUP MALAYSIA', 'Industries': 'Market Research', 'start_date': '2022-05', 'end_date': '2022-09', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'R&amp;D and QC Chemist', 'job_company': 'SMART INK SDN BHD', 'Industries': 'Chemical', 'start_date': '2021-04', 'end_date': '2022-04', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Research Assistant Intern', 'job_company': 'UNIVERSITI PUTRA MALAYSIA', 'Industries': 'Research', 'start_date': '2019-06', 'end_date': '2019-09', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[['Electric, Electronics &amp; System Engineering (Image processing)', 'Master of Science', 'N/A', 'Universiti Kebangsaan Malaysia', '2015-2019'], ['Electric, Electronics &amp; System Engineering (Communication &amp; Computer)', "Bachelor's degree", 'N/A', 'Universiti Kebangsaan Malaysia', '2009-2013'], ['Science majoring in Biology', 'Matriculation', 'N/A', 'Penang Matriculation College', '2008-2009']]</t>
+          <t>[{'Country': 'N/A', 'State': 'N/A', 'City': 'N/A'}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['Google Data Analytics Professional Certificate']</t>
+          <t>[{'field_of_study': 'Applied Chemistry', 'level': "Bachelor's", 'cgpa': 'N/A', 'university': 'Universiti Teknologi MARA', 'start_date': '2017', 'year_of_graduation': '2021'}]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['SQL', 'R (Programming Language)', 'Data Analytics', 'Project Planning', 'Google Sheets', 'Data Analysis', 'Research and Development (R&amp;D)', 'Professional Communication', 'Program Management', 'C (Programming Language)']</t>
+          <t>['Zero Microsoft Excel Complete 2020', 'Google Data Analytics', 'Data Star Program Data Analyst']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['MATLAB', 'Python', 'R', 'SQL', 'Microsoft Word', 'Microsoft PowerPoint', 'Microsoft Excel', 'Microsoft Access', 'Microsoft Publisher', 'Google Docs', 'Google Sheets', 'Google Slides', 'Google Form', 'MPLAB', 'Arduino IDE', 'Visual Studio Code IDE', 'MIT App Inventor', 'Filmora 9', 'SPSS']</t>
+          <t>['Microsoft Word', 'Microsoft Excel', 'Microsoft PowerPoint', 'C++ Programming Language', 'Microsoft Outlook', 'ChemDraw', 'Microsoft Access', 'Python Programming Language', 'SQL', 'Tableau']</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['N/A']</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>[{'job_title': 'Media Officer', 'job_company': 'Pertubuhan IKRAM Malaysia', 'Industries': 'Media', 'start_date': '2021-04', 'end_date': 'Present', 'job_location': 'N/A', 'job_duration': 1.92}, {'job_title': 'Research Officer', 'job_company': 'UKM', 'Industries': 'Research', 'start_date': '2019-04', 'end_date': '2020-08', 'job_location': 'N/A', 'job_duration': 1.42}, {'job_title': 'Research Assistant', 'job_company': 'UKM', 'Industries': 'Research', 'start_date': '2014-04', 'end_date': '2015-07', 'job_location': 'N/A', 'job_duration': 1.33}, {'job_title': 'Internship', 'job_company': 'Astana Digital Sdn. Bhd', 'Industries': 'N/A', 'start_date': '2012-06', 'end_date': '2012-09', 'job_location': 'N/A', 'job_duration': 0.33}]</t>
+          <t>['Bahasa Melayu', 'English', 'Bahasa Indonesia', 'Japanese', 'Arabic']</t>
         </is>
       </c>
     </row>
@@ -566,17 +556,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ELNI FATIENY BINTI MOHD SALMI</t>
+          <t>Nafhan Najib</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>011-13244806</t>
+          <t>+60-127445518</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>elnifatieny136@gmail.com</t>
+          <t>nafhannajib@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -591,37 +581,32 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['Malaysia', 'N/A', 'N/A']</t>
+          <t>[{'job_title': 'Region Leader', 'job_company': 'Foxconn Vietnam plant', 'Industries': 'N/A', 'start_date': 'N/A', 'end_date': 'N/A', 'job_location': 'Kajang, Selangor', 'job_duration': 'N/A'}, {'job_title': 'Sony Green Partner Auditor', 'job_company': 'N/A', 'Industries': 'N/A', 'start_date': 'N/A', 'end_date': 'N/A', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Electrical Model Leader', 'job_company': 'KIT Plant (Egypt)', 'Industries': 'N/A', 'start_date': 'N/A', 'end_date': 'N/A', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Senior Design Engineer (Project)', 'job_company': 'Sony EMCS (M) Sdn Bhd', 'Industries': 'N/A', 'start_date': 'Dec 2018', 'end_date': 'Present', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Intern', 'job_company': 'AEM Microtronics Sdn Bhd', 'Industries': 'N/A', 'start_date': 'Feb 2018', 'end_date': 'Jun 2018', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'Intern', 'job_company': 'Hospital Sultanah Bahiyah', 'Industries': 'N/A', 'start_date': 'Jul 2017', 'end_date': 'Aug 2017', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Information System', 'level': 'Bachelor of Science', 'cgpa': '3.53', 'university': 'Universiti Teknologi Petronas', 'start_date': '2018-05', 'year_of_graduation': '2021'}]</t>
+          <t>[{'Country': 'N/A', 'State': 'N/A', 'City': 'N/A'}]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>[{'field_of_study': 'Physics', 'level': 'Bachelor of Science', 'cgpa': '3.45', 'university': 'Universiti Sains Malaysia', 'start_date': '2015', 'year_of_graduation': '2018'}, {'field_of_study': 'Innovation &amp; Engineering Design', 'level': 'Master of Science', 'cgpa': '3.94', 'university': 'Universiti Putra Malaysia', 'start_date': '2019', 'year_of_graduation': '2020'}]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>['N/A']</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>['Data Analyst', 'Corporate Management', 'Software Designing', 'Project Management', 'Marketing Operation']</t>
-        </is>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>['Eclipse', 'Anaconda', 'R studio', 'Android Studio', 'PowerBI', 'Firebase', 'Visual Studio Code', 'Microsoft Office', 'Google Collab', 'Oracle Live', 'phpMyAdmin', 'MySQL', 'SQL Server Management Studio', 'WinSCP', 'Salesforce', 'WordPress']</t>
+          <t>['Python', 'Visual Basic for Application (VBA)', 'C++', 'Microsoft Power BI', 'Solidworks', 'Applied Data Engineer', 'Google Project Management', 'Digital Leadership Development', 'Python 3 Programming']</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>['Malay', 'English']</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>[{'job_title': 'Marketing Associate Operation', 'job_company': '2X Marketing Sdn Bhd', 'Industries': 'Marketing', 'start_date': '2022-09', 'end_date': '2024-05-15'}, {'job_title': 'Software Engineer', 'job_company': 'ManagePay System Berhad', 'Industries': 'Finance', 'start_date': '2022-01', 'end_date': '2024-05-15'}, {'job_title': 'Change Management Intern', 'job_company': 'Petroliam Nasional Berhad', 'Industries': 'Oil &amp; Gas', 'start_date': '2020-01', 'end_date': '2020-09'}]</t>
+          <t>['Malay', 'English', 'Mandarin', 'Spanish']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add format field to current location, add format field to post evaluation results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -496,17 +496,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kelvin Ee</t>
+          <t>ADAM SYAFIQ BIN SAFIAN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+60 11-3919 0131</t>
+          <t>011-25686811</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>kelvinee2001@gmail.com</t>
+          <t>adamsyafiq31@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{'job_title': 'PHP Web Developer', 'job_company': 'Powerec Services Sdn Bhd', 'Industries': 'N/A', 'start_date': '2021-11', 'end_date': '2022-02', 'job_location': 'N/A', 'job_duration': 'N/A'}, {'job_title': 'PPG Intern', 'job_company': 'N/A', 'Industries': 'N/A', 'start_date': '2023-08', 'end_date': '2024-05-19 11:33:54.994675', 'job_location': 'N/A', 'job_duration': 'N/A'}]</t>
+          <t>[{'job_title': 'Document Controller', 'job_company': 'China Communication Construction (ECRL) Sdn Bhd', 'Industries': 'N/A', 'start_date': '2022-01', 'end_date': '2024-05-21 02:50:37.826879', 'job_location': 'N/A', 'job_duration': '2 years 4 months'}]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -531,22 +531,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[{'field_of_study': 'Bachelor of Computer Science (Data Engineering)', 'level': "Bachelor's Degree", 'cgpa': '3.98', 'university': 'Universiti Teknologi Malaysia', 'start_date': '2020', 'year_of_graduation': 'N/A'}]</t>
+          <t>[{'field_of_study': 'Bachelor in Engineering Technology (Facilities Maintenance Engineering)', 'level': "Bachelor's Degree", 'cgpa': 'N/A', 'university': 'UniKL Mitec', 'start_date': '2018', 'year_of_graduation': '2021'}, {'field_of_study': 'Diploma in Construction Technology (Building Services and Maintenance)', 'level': 'Diploma', 'cgpa': 'N/A', 'university': 'KKTM Sri Gading', 'start_date': '2015', 'year_of_graduation': '2018'}]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['Alteryx Designer Core Certified']</t>
+          <t>['N/A']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['Python', 'SQL', 'C++', 'R', 'Power BI', 'Tableau', 'Alteryx', 'Excel', 'Databricks', 'Azure Data Factory', 'Blob Storage', 'KeyVault', 'HTML', 'CSS', 'PHP', 'Bootstrap', 'JavaScript', 'C#', 'Cloud Foundation', 'Machine Learning', 'Data Analytic']</t>
+          <t>['Teamwork', 'Time Management', 'Leadership', 'Microsoft Office', 'Bahasa Malaysia']</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>['English', 'Malay', 'Chinese']</t>
+          <t>['Mandarin', 'English']</t>
         </is>
       </c>
     </row>

</xml_diff>